<commit_message>
Add template inspection log
</commit_message>
<xml_diff>
--- a/dist/modules/data/templates/Incoming Inspection Log.xlsx
+++ b/dist/modules/data/templates/Incoming Inspection Log.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\austi\Documents\Pragmatic\Projects\DBA-Automation-Tools\dist\modules\data\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1D6F6255-207D-4310-B2CC-8523CB905123}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FE3C4C9-A680-4E60-AF05-36A64BD54E38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5235" yWindow="2700" windowWidth="19380" windowHeight="12045" xr2:uid="{787A15B7-D0B2-4895-82D1-FA4613D51671}"/>
+    <workbookView xWindow="4560" yWindow="1380" windowWidth="19380" windowHeight="12045" xr2:uid="{787A15B7-D0B2-4895-82D1-FA4613D51671}"/>
   </bookViews>
   <sheets>
     <sheet name="Incoming Log 2020" sheetId="2" r:id="rId1"/>
     <sheet name="Revision History" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Incoming Log 2020'!$A$2:$I$75</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Incoming Log 2020'!$A$1:$I$75</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Incoming Log 2020'!$A$2:$J$75</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Incoming Log 2020'!$A$1:$J$75</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="38">
   <si>
     <t>Incoming Inspection Log</t>
   </si>
@@ -107,6 +107,51 @@
   </si>
   <si>
     <t>Accept or Reject</t>
+  </si>
+  <si>
+    <t>Inspection Number</t>
+  </si>
+  <si>
+    <t>Sample Part Description</t>
+  </si>
+  <si>
+    <t>PO11796</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>CC106014170 S470.1, ETFE 25%GF</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -689,6 +734,20 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
@@ -696,20 +755,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1028,11 +1073,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AA75"/>
+  <dimension ref="A1:AB75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1040,24 +1085,25 @@
     <col min="1" max="2" width="18.7109375" customWidth="1"/>
     <col min="3" max="3" width="50.7109375" customWidth="1"/>
     <col min="4" max="4" width="30.7109375" customWidth="1"/>
-    <col min="5" max="9" width="12.7109375" customWidth="1"/>
-    <col min="10" max="22" width="11.7109375" customWidth="1"/>
+    <col min="5" max="10" width="12.7109375" customWidth="1"/>
+    <col min="11" max="23" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+    <row r="1" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="47"/>
-    </row>
-    <row r="2" spans="1:27" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="40"/>
+    </row>
+    <row r="2" spans="1:28" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -1077,15 +1123,17 @@
         <v>5</v>
       </c>
       <c r="G2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="29" t="s">
+      <c r="I2" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
@@ -1099,834 +1147,1436 @@
       <c r="U2" s="1"/>
       <c r="V2" s="1"/>
       <c r="W2" s="1"/>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="20"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="23"/>
-      <c r="AA3" t="s">
+      <c r="X2" s="1"/>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>44927</v>
+      </c>
+      <c r="B3" s="20">
+        <v>100636</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="33">
+        <v>123456</v>
+      </c>
+      <c r="E3" s="21">
+        <v>20</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="30"/>
+      <c r="J3" s="23"/>
+      <c r="AB3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="27"/>
-      <c r="AA4" t="s">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>44927</v>
+      </c>
+      <c r="B4" s="24">
+        <v>100636</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="34">
+        <v>123456</v>
+      </c>
+      <c r="E4" s="25">
+        <v>20</v>
+      </c>
+      <c r="F4" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="31"/>
+      <c r="J4" s="27"/>
+      <c r="AB4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="24"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="31"/>
-      <c r="I5" s="27"/>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="24"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="27"/>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="24"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="27"/>
-      <c r="AA7" t="s">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>44927</v>
+      </c>
+      <c r="B5" s="24">
+        <v>100636</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="35">
+        <v>123456</v>
+      </c>
+      <c r="E5" s="25">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="24"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="31"/>
-      <c r="I8" s="27"/>
-      <c r="AA8" t="s">
+      <c r="F5" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" s="31"/>
+      <c r="J5" s="27"/>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>44927</v>
+      </c>
+      <c r="B6" s="24">
+        <v>100636</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="34">
+        <v>123456</v>
+      </c>
+      <c r="E6" s="25">
+        <v>20</v>
+      </c>
+      <c r="F6" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" s="31"/>
+      <c r="J6" s="27"/>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>44927</v>
+      </c>
+      <c r="B7" s="24">
+        <v>100636</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="34">
+        <v>123456</v>
+      </c>
+      <c r="E7" s="25">
+        <v>20</v>
+      </c>
+      <c r="F7" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="I7" s="31"/>
+      <c r="J7" s="27"/>
+      <c r="AB7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>44927</v>
+      </c>
+      <c r="B8" s="24">
+        <v>100636</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="34">
+        <v>123456</v>
+      </c>
+      <c r="E8" s="25">
+        <v>20</v>
+      </c>
+      <c r="F8" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="I8" s="31"/>
+      <c r="J8" s="27"/>
+      <c r="AB8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="24"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="31"/>
-      <c r="I9" s="27"/>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="24"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="26"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="27"/>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="31"/>
-      <c r="I11" s="27"/>
-    </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="24"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="31"/>
-      <c r="I12" s="27"/>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="24"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="34"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="31"/>
-      <c r="I13" s="27"/>
-    </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="24"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="34"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="31"/>
-      <c r="I14" s="27"/>
-    </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="34"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="31"/>
-      <c r="I15" s="27"/>
-    </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="24"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="31"/>
-      <c r="I16" s="27"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="24"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="31"/>
-      <c r="I17" s="27"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="24"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="31"/>
-      <c r="I18" s="27"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-      <c r="B19" s="24"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="31"/>
-      <c r="I19" s="27"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="B20" s="24"/>
-      <c r="C20" s="25"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="26"/>
-      <c r="H20" s="31"/>
-      <c r="I20" s="27"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" s="24"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="34"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="31"/>
-      <c r="I21" s="27"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-      <c r="B22" s="24"/>
-      <c r="C22" s="25"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="31"/>
-      <c r="I22" s="27"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
-      <c r="B23" s="24"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="34"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="26"/>
-      <c r="H23" s="31"/>
-      <c r="I23" s="27"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
-      <c r="B24" s="24"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="34"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="31"/>
-      <c r="I24" s="27"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
-      <c r="B25" s="24"/>
-      <c r="C25" s="25"/>
-      <c r="D25" s="34"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="25"/>
-      <c r="G25" s="26"/>
-      <c r="H25" s="31"/>
-      <c r="I25" s="27"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
-      <c r="B26" s="24"/>
-      <c r="C26" s="25"/>
-      <c r="D26" s="34"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="25"/>
-      <c r="G26" s="26"/>
-      <c r="H26" s="31"/>
-      <c r="I26" s="27"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="3"/>
-      <c r="B27" s="24"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="25"/>
-      <c r="G27" s="26"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="27"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="3"/>
-      <c r="B28" s="24"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="34"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="26"/>
-      <c r="H28" s="31"/>
-      <c r="I28" s="27"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="3"/>
-      <c r="B29" s="24"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="34"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="31"/>
-      <c r="I29" s="27"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="3"/>
-      <c r="B30" s="24"/>
-      <c r="C30" s="25"/>
-      <c r="D30" s="34"/>
-      <c r="E30" s="25"/>
-      <c r="F30" s="25"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="31"/>
-      <c r="I30" s="27"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="3"/>
-      <c r="B31" s="28"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="34"/>
-      <c r="E31" s="25"/>
-      <c r="F31" s="25"/>
-      <c r="G31" s="26"/>
-      <c r="H31" s="31"/>
-      <c r="I31" s="27"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="3"/>
-      <c r="B32" s="24"/>
-      <c r="C32" s="25"/>
-      <c r="D32" s="34"/>
-      <c r="E32" s="25"/>
-      <c r="F32" s="25"/>
-      <c r="G32" s="26"/>
-      <c r="H32" s="31"/>
-      <c r="I32" s="27"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="3"/>
-      <c r="B33" s="24"/>
-      <c r="C33" s="32"/>
-      <c r="D33" s="34"/>
-      <c r="E33" s="25"/>
-      <c r="F33" s="25"/>
-      <c r="G33" s="26"/>
-      <c r="H33" s="31"/>
-      <c r="I33" s="27"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="3"/>
-      <c r="B34" s="24"/>
-      <c r="C34" s="32"/>
-      <c r="D34" s="34"/>
-      <c r="E34" s="25"/>
-      <c r="F34" s="25"/>
-      <c r="G34" s="26"/>
-      <c r="H34" s="31"/>
-      <c r="I34" s="27"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="3"/>
-      <c r="B35" s="24"/>
-      <c r="C35" s="25"/>
-      <c r="D35" s="34"/>
-      <c r="E35" s="25"/>
-      <c r="F35" s="25"/>
-      <c r="G35" s="26"/>
-      <c r="H35" s="31"/>
-      <c r="I35" s="27"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>44927</v>
+      </c>
+      <c r="B9" s="24">
+        <v>100636</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="34">
+        <v>123456</v>
+      </c>
+      <c r="E9" s="25">
+        <v>20</v>
+      </c>
+      <c r="F9" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="I9" s="31"/>
+      <c r="J9" s="27"/>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>44927</v>
+      </c>
+      <c r="B10" s="24">
+        <v>100636</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="34">
+        <v>123456</v>
+      </c>
+      <c r="E10" s="25">
+        <v>20</v>
+      </c>
+      <c r="F10" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="I10" s="31"/>
+      <c r="J10" s="27"/>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>44927</v>
+      </c>
+      <c r="B11" s="24">
+        <v>100636</v>
+      </c>
+      <c r="C11" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="34">
+        <v>123456</v>
+      </c>
+      <c r="E11" s="25">
+        <v>20</v>
+      </c>
+      <c r="F11" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="I11" s="31"/>
+      <c r="J11" s="27"/>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>44927</v>
+      </c>
+      <c r="B12" s="24">
+        <v>100636</v>
+      </c>
+      <c r="C12" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="34">
+        <v>123456</v>
+      </c>
+      <c r="E12" s="25">
+        <v>20</v>
+      </c>
+      <c r="F12" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="H12" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="I12" s="31"/>
+      <c r="J12" s="27"/>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>44927</v>
+      </c>
+      <c r="B13" s="24">
+        <v>100636</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="34">
+        <v>123456</v>
+      </c>
+      <c r="E13" s="25">
+        <v>20</v>
+      </c>
+      <c r="F13" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="H13" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="I13" s="31"/>
+      <c r="J13" s="27"/>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>44927</v>
+      </c>
+      <c r="B14" s="24">
+        <v>100636</v>
+      </c>
+      <c r="C14" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="34">
+        <v>123456</v>
+      </c>
+      <c r="E14" s="25">
+        <v>20</v>
+      </c>
+      <c r="F14" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="G14" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="H14" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="I14" s="31"/>
+      <c r="J14" s="27"/>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>44927</v>
+      </c>
+      <c r="B15" s="24">
+        <v>100636</v>
+      </c>
+      <c r="C15" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="34">
+        <v>123456</v>
+      </c>
+      <c r="E15" s="25">
+        <v>20</v>
+      </c>
+      <c r="F15" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="G15" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="H15" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="I15" s="31"/>
+      <c r="J15" s="27"/>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>44927</v>
+      </c>
+      <c r="B16" s="24">
+        <v>100636</v>
+      </c>
+      <c r="C16" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="34">
+        <v>123456</v>
+      </c>
+      <c r="E16" s="25">
+        <v>20</v>
+      </c>
+      <c r="F16" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="G16" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="H16" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="I16" s="31"/>
+      <c r="J16" s="27"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>44927</v>
+      </c>
+      <c r="B17" s="24">
+        <v>100636</v>
+      </c>
+      <c r="C17" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="34">
+        <v>123456</v>
+      </c>
+      <c r="E17" s="25">
+        <v>20</v>
+      </c>
+      <c r="F17" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="G17" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="H17" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="I17" s="31"/>
+      <c r="J17" s="27"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>44927</v>
+      </c>
+      <c r="B18" s="24">
+        <v>100636</v>
+      </c>
+      <c r="C18" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="34">
+        <v>123456</v>
+      </c>
+      <c r="E18" s="25">
+        <v>20</v>
+      </c>
+      <c r="F18" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="G18" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="H18" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="I18" s="31"/>
+      <c r="J18" s="27"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>44927</v>
+      </c>
+      <c r="B19" s="24">
+        <v>100636</v>
+      </c>
+      <c r="C19" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="34">
+        <v>123456</v>
+      </c>
+      <c r="E19" s="25">
+        <v>20</v>
+      </c>
+      <c r="F19" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="G19" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="H19" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="I19" s="31"/>
+      <c r="J19" s="27"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>44927</v>
+      </c>
+      <c r="B20" s="24">
+        <v>100636</v>
+      </c>
+      <c r="C20" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" s="34">
+        <v>123456</v>
+      </c>
+      <c r="E20" s="25">
+        <v>20</v>
+      </c>
+      <c r="F20" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="G20" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="H20" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="I20" s="31"/>
+      <c r="J20" s="27"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>44927</v>
+      </c>
+      <c r="B21" s="24">
+        <v>100636</v>
+      </c>
+      <c r="C21" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" s="34">
+        <v>123456</v>
+      </c>
+      <c r="E21" s="25">
+        <v>20</v>
+      </c>
+      <c r="F21" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="G21" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="H21" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="I21" s="31"/>
+      <c r="J21" s="27"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>44927</v>
+      </c>
+      <c r="B22" s="24">
+        <v>100636</v>
+      </c>
+      <c r="C22" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="34">
+        <v>123456</v>
+      </c>
+      <c r="E22" s="25">
+        <v>20</v>
+      </c>
+      <c r="F22" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="G22" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="H22" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="I22" s="31"/>
+      <c r="J22" s="27"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>44927</v>
+      </c>
+      <c r="B23" s="24">
+        <v>100636</v>
+      </c>
+      <c r="C23" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" s="34">
+        <v>123456</v>
+      </c>
+      <c r="E23" s="25">
+        <v>20</v>
+      </c>
+      <c r="F23" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="G23" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="H23" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="I23" s="31"/>
+      <c r="J23" s="27"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>44927</v>
+      </c>
+      <c r="B24" s="24">
+        <v>100636</v>
+      </c>
+      <c r="C24" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" s="34">
+        <v>123456</v>
+      </c>
+      <c r="E24" s="25">
+        <v>20</v>
+      </c>
+      <c r="F24" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="G24" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="H24" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="I24" s="31"/>
+      <c r="J24" s="27"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>44927</v>
+      </c>
+      <c r="B25" s="24">
+        <v>100636</v>
+      </c>
+      <c r="C25" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="D25" s="34">
+        <v>123456</v>
+      </c>
+      <c r="E25" s="25">
+        <v>20</v>
+      </c>
+      <c r="F25" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="G25" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="H25" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="I25" s="31"/>
+      <c r="J25" s="27"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>44927</v>
+      </c>
+      <c r="B26" s="24">
+        <v>100636</v>
+      </c>
+      <c r="C26" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="D26" s="34">
+        <v>123456</v>
+      </c>
+      <c r="E26" s="25">
+        <v>20</v>
+      </c>
+      <c r="F26" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="G26" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="H26" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="I26" s="31"/>
+      <c r="J26" s="27"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>44951</v>
+      </c>
+      <c r="B27" s="24">
+        <v>100636</v>
+      </c>
+      <c r="C27" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="D27" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="E27" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="F27" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="G27" s="25">
+        <v>100029</v>
+      </c>
+      <c r="H27" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="I27" s="31"/>
+      <c r="J27" s="27"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>44951</v>
+      </c>
+      <c r="B28" s="24">
+        <v>100636</v>
+      </c>
+      <c r="C28" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="E28" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="F28" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="G28" s="25">
+        <v>100030</v>
+      </c>
+      <c r="H28" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="I28" s="31"/>
+      <c r="J28" s="27"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>44951</v>
+      </c>
+      <c r="B29" s="24">
+        <v>100636</v>
+      </c>
+      <c r="C29" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="E29" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="F29" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="G29" s="25">
+        <v>100031</v>
+      </c>
+      <c r="H29" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="I29" s="31"/>
+      <c r="J29" s="27"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>44951</v>
+      </c>
+      <c r="B30" s="24">
+        <v>100636</v>
+      </c>
+      <c r="C30" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="D30" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="E30" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="F30" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="G30" s="25">
+        <v>100041</v>
+      </c>
+      <c r="H30" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="I30" s="31"/>
+      <c r="J30" s="27"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>44951</v>
+      </c>
+      <c r="B31" s="28">
+        <v>100636</v>
+      </c>
+      <c r="C31" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="D31" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="E31" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="F31" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="G31" s="25">
+        <v>100042</v>
+      </c>
+      <c r="H31" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="I31" s="31"/>
+      <c r="J31" s="27"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>44951</v>
+      </c>
+      <c r="B32" s="24">
+        <v>100636</v>
+      </c>
+      <c r="C32" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="D32" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="E32" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="F32" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="G32" s="25">
+        <v>100043</v>
+      </c>
+      <c r="H32" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="I32" s="31"/>
+      <c r="J32" s="27"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>44951</v>
+      </c>
+      <c r="B33" s="24">
+        <v>100636</v>
+      </c>
+      <c r="C33" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="D33" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="E33" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="F33" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="G33" s="25">
+        <v>100044</v>
+      </c>
+      <c r="H33" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="I33" s="31"/>
+      <c r="J33" s="27"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>44951</v>
+      </c>
+      <c r="B34" s="24">
+        <v>100636</v>
+      </c>
+      <c r="C34" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="D34" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="E34" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="F34" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="G34" s="25">
+        <v>100045</v>
+      </c>
+      <c r="H34" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="I34" s="31"/>
+      <c r="J34" s="27"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>44951</v>
+      </c>
+      <c r="B35" s="24">
+        <v>100636</v>
+      </c>
+      <c r="C35" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="D35" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="E35" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="F35" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="G35" s="25">
+        <v>100046</v>
+      </c>
+      <c r="H35" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="I35" s="31"/>
+      <c r="J35" s="27"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="24"/>
       <c r="C36" s="25"/>
       <c r="D36" s="34"/>
       <c r="E36" s="25"/>
       <c r="F36" s="25"/>
-      <c r="G36" s="26"/>
-      <c r="H36" s="31"/>
-      <c r="I36" s="27"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G36" s="25"/>
+      <c r="H36" s="26"/>
+      <c r="I36" s="31"/>
+      <c r="J36" s="27"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="24"/>
       <c r="C37" s="25"/>
       <c r="D37" s="34"/>
       <c r="E37" s="25"/>
       <c r="F37" s="25"/>
-      <c r="G37" s="26"/>
-      <c r="H37" s="31"/>
-      <c r="I37" s="27"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G37" s="25"/>
+      <c r="H37" s="26"/>
+      <c r="I37" s="31"/>
+      <c r="J37" s="27"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="24"/>
       <c r="C38" s="25"/>
       <c r="D38" s="34"/>
       <c r="E38" s="25"/>
       <c r="F38" s="25"/>
-      <c r="G38" s="26"/>
-      <c r="H38" s="31"/>
-      <c r="I38" s="27"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G38" s="25"/>
+      <c r="H38" s="26"/>
+      <c r="I38" s="31"/>
+      <c r="J38" s="27"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
       <c r="B39" s="24"/>
       <c r="C39" s="25"/>
       <c r="D39" s="34"/>
       <c r="E39" s="25"/>
       <c r="F39" s="25"/>
-      <c r="G39" s="26"/>
-      <c r="H39" s="31"/>
-      <c r="I39" s="27"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G39" s="25"/>
+      <c r="H39" s="26"/>
+      <c r="I39" s="31"/>
+      <c r="J39" s="27"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
       <c r="B40" s="24"/>
       <c r="C40" s="25"/>
       <c r="D40" s="34"/>
       <c r="E40" s="25"/>
       <c r="F40" s="25"/>
-      <c r="G40" s="26"/>
-      <c r="H40" s="31"/>
-      <c r="I40" s="27"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G40" s="25"/>
+      <c r="H40" s="26"/>
+      <c r="I40" s="31"/>
+      <c r="J40" s="27"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
       <c r="B41" s="24"/>
       <c r="C41" s="25"/>
       <c r="D41" s="34"/>
       <c r="E41" s="25"/>
       <c r="F41" s="25"/>
-      <c r="G41" s="26"/>
-      <c r="H41" s="31"/>
-      <c r="I41" s="27"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G41" s="25"/>
+      <c r="H41" s="26"/>
+      <c r="I41" s="31"/>
+      <c r="J41" s="27"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="24"/>
       <c r="C42" s="32"/>
       <c r="D42" s="34"/>
       <c r="E42" s="25"/>
       <c r="F42" s="25"/>
-      <c r="G42" s="26"/>
-      <c r="H42" s="31"/>
-      <c r="I42" s="27"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G42" s="25"/>
+      <c r="H42" s="26"/>
+      <c r="I42" s="31"/>
+      <c r="J42" s="27"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
       <c r="B43" s="24"/>
       <c r="C43" s="25"/>
       <c r="D43" s="35"/>
       <c r="E43" s="25"/>
       <c r="F43" s="25"/>
-      <c r="G43" s="26"/>
-      <c r="H43" s="31"/>
-      <c r="I43" s="27"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G43" s="25"/>
+      <c r="H43" s="26"/>
+      <c r="I43" s="31"/>
+      <c r="J43" s="27"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
       <c r="B44" s="24"/>
       <c r="C44" s="25"/>
       <c r="D44" s="34"/>
       <c r="E44" s="25"/>
       <c r="F44" s="25"/>
-      <c r="G44" s="26"/>
-      <c r="H44" s="31"/>
-      <c r="I44" s="27"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G44" s="25"/>
+      <c r="H44" s="26"/>
+      <c r="I44" s="31"/>
+      <c r="J44" s="27"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
       <c r="B45" s="24"/>
       <c r="C45" s="25"/>
       <c r="D45" s="34"/>
       <c r="E45" s="25"/>
       <c r="F45" s="25"/>
-      <c r="G45" s="26"/>
-      <c r="H45" s="31"/>
-      <c r="I45" s="27"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G45" s="25"/>
+      <c r="H45" s="26"/>
+      <c r="I45" s="31"/>
+      <c r="J45" s="27"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
       <c r="B46" s="24"/>
       <c r="C46" s="25"/>
       <c r="D46" s="34"/>
       <c r="E46" s="25"/>
       <c r="F46" s="25"/>
-      <c r="G46" s="26"/>
-      <c r="H46" s="31"/>
-      <c r="I46" s="27"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G46" s="25"/>
+      <c r="H46" s="26"/>
+      <c r="I46" s="31"/>
+      <c r="J46" s="27"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
       <c r="B47" s="24"/>
       <c r="C47" s="25"/>
       <c r="D47" s="34"/>
       <c r="E47" s="25"/>
       <c r="F47" s="25"/>
-      <c r="G47" s="26"/>
-      <c r="H47" s="31"/>
-      <c r="I47" s="27"/>
-    </row>
-    <row r="48" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G47" s="25"/>
+      <c r="H47" s="26"/>
+      <c r="I47" s="31"/>
+      <c r="J47" s="27"/>
+    </row>
+    <row r="48" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
       <c r="B48" s="24"/>
       <c r="C48" s="32"/>
       <c r="D48" s="34"/>
       <c r="E48" s="25"/>
       <c r="F48" s="25"/>
-      <c r="G48" s="26"/>
-      <c r="H48" s="31"/>
-      <c r="I48" s="27"/>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G48" s="25"/>
+      <c r="H48" s="26"/>
+      <c r="I48" s="31"/>
+      <c r="J48" s="27"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="3"/>
       <c r="B49" s="24"/>
       <c r="C49" s="25"/>
       <c r="D49" s="36"/>
       <c r="E49" s="25"/>
       <c r="F49" s="25"/>
-      <c r="G49" s="26"/>
-      <c r="H49" s="31"/>
-      <c r="I49" s="27"/>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G49" s="25"/>
+      <c r="H49" s="26"/>
+      <c r="I49" s="31"/>
+      <c r="J49" s="27"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
       <c r="B50" s="24"/>
       <c r="C50" s="32"/>
       <c r="D50" s="35"/>
       <c r="E50" s="25"/>
       <c r="F50" s="25"/>
-      <c r="G50" s="26"/>
-      <c r="H50" s="31"/>
-      <c r="I50" s="27"/>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G50" s="25"/>
+      <c r="H50" s="26"/>
+      <c r="I50" s="31"/>
+      <c r="J50" s="27"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="3"/>
       <c r="B51" s="24"/>
       <c r="C51" s="25"/>
       <c r="D51" s="34"/>
       <c r="E51" s="25"/>
       <c r="F51" s="25"/>
-      <c r="G51" s="26"/>
-      <c r="H51" s="31"/>
-      <c r="I51" s="27"/>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G51" s="25"/>
+      <c r="H51" s="26"/>
+      <c r="I51" s="31"/>
+      <c r="J51" s="27"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
       <c r="B52" s="24"/>
       <c r="C52" s="25"/>
       <c r="D52" s="34"/>
       <c r="E52" s="25"/>
       <c r="F52" s="25"/>
-      <c r="G52" s="26"/>
-      <c r="H52" s="31"/>
-      <c r="I52" s="27"/>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G52" s="25"/>
+      <c r="H52" s="26"/>
+      <c r="I52" s="31"/>
+      <c r="J52" s="27"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="3"/>
       <c r="B53" s="24"/>
       <c r="C53" s="25"/>
       <c r="D53" s="36"/>
       <c r="E53" s="25"/>
       <c r="F53" s="25"/>
-      <c r="G53" s="26"/>
-      <c r="H53" s="31"/>
-      <c r="I53" s="27"/>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G53" s="25"/>
+      <c r="H53" s="26"/>
+      <c r="I53" s="31"/>
+      <c r="J53" s="27"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="3"/>
       <c r="B54" s="24"/>
       <c r="C54" s="25"/>
       <c r="D54" s="36"/>
       <c r="E54" s="25"/>
       <c r="F54" s="25"/>
-      <c r="G54" s="26"/>
-      <c r="H54" s="31"/>
-      <c r="I54" s="27"/>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G54" s="25"/>
+      <c r="H54" s="26"/>
+      <c r="I54" s="31"/>
+      <c r="J54" s="27"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="3"/>
       <c r="B55" s="24"/>
       <c r="C55" s="25"/>
       <c r="D55" s="36"/>
       <c r="E55" s="25"/>
       <c r="F55" s="25"/>
-      <c r="G55" s="26"/>
-      <c r="H55" s="31"/>
-      <c r="I55" s="27"/>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G55" s="25"/>
+      <c r="H55" s="26"/>
+      <c r="I55" s="31"/>
+      <c r="J55" s="27"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>
       <c r="B56" s="24"/>
       <c r="C56" s="25"/>
       <c r="D56" s="35"/>
       <c r="E56" s="25"/>
       <c r="F56" s="25"/>
-      <c r="G56" s="26"/>
-      <c r="H56" s="31"/>
-      <c r="I56" s="27"/>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G56" s="25"/>
+      <c r="H56" s="26"/>
+      <c r="I56" s="31"/>
+      <c r="J56" s="27"/>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="3"/>
       <c r="B57" s="24"/>
       <c r="C57" s="25"/>
       <c r="D57" s="36"/>
       <c r="E57" s="25"/>
       <c r="F57" s="25"/>
-      <c r="G57" s="26"/>
-      <c r="H57" s="31"/>
-      <c r="I57" s="27"/>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G57" s="25"/>
+      <c r="H57" s="26"/>
+      <c r="I57" s="31"/>
+      <c r="J57" s="27"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="3"/>
       <c r="B58" s="24"/>
       <c r="C58" s="25"/>
       <c r="D58" s="36"/>
       <c r="E58" s="25"/>
       <c r="F58" s="25"/>
-      <c r="G58" s="26"/>
-      <c r="H58" s="31"/>
-      <c r="I58" s="27"/>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G58" s="25"/>
+      <c r="H58" s="26"/>
+      <c r="I58" s="31"/>
+      <c r="J58" s="27"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="3"/>
       <c r="B59" s="24"/>
       <c r="C59" s="25"/>
       <c r="D59" s="36"/>
       <c r="E59" s="25"/>
       <c r="F59" s="25"/>
-      <c r="G59" s="26"/>
-      <c r="H59" s="31"/>
-      <c r="I59" s="27"/>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G59" s="25"/>
+      <c r="H59" s="26"/>
+      <c r="I59" s="31"/>
+      <c r="J59" s="27"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="3"/>
       <c r="B60" s="24"/>
       <c r="C60" s="25"/>
       <c r="D60" s="36"/>
       <c r="E60" s="25"/>
       <c r="F60" s="25"/>
-      <c r="G60" s="26"/>
-      <c r="H60" s="31"/>
-      <c r="I60" s="27"/>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G60" s="25"/>
+      <c r="H60" s="26"/>
+      <c r="I60" s="31"/>
+      <c r="J60" s="27"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="3"/>
       <c r="B61" s="24"/>
       <c r="C61" s="25"/>
       <c r="D61" s="35"/>
       <c r="E61" s="25"/>
       <c r="F61" s="25"/>
-      <c r="G61" s="26"/>
-      <c r="H61" s="31"/>
-      <c r="I61" s="27"/>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G61" s="25"/>
+      <c r="H61" s="26"/>
+      <c r="I61" s="31"/>
+      <c r="J61" s="27"/>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="3"/>
       <c r="B62" s="24"/>
       <c r="C62" s="25"/>
       <c r="D62" s="36"/>
       <c r="E62" s="25"/>
       <c r="F62" s="25"/>
-      <c r="G62" s="26"/>
-      <c r="H62" s="31"/>
-      <c r="I62" s="27"/>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G62" s="25"/>
+      <c r="H62" s="26"/>
+      <c r="I62" s="31"/>
+      <c r="J62" s="27"/>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="3"/>
       <c r="B63" s="24"/>
       <c r="C63" s="25"/>
       <c r="D63" s="36"/>
       <c r="E63" s="25"/>
       <c r="F63" s="25"/>
-      <c r="G63" s="26"/>
-      <c r="H63" s="31"/>
-      <c r="I63" s="27"/>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G63" s="25"/>
+      <c r="H63" s="26"/>
+      <c r="I63" s="31"/>
+      <c r="J63" s="27"/>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="3"/>
       <c r="B64" s="24"/>
       <c r="C64" s="25"/>
       <c r="D64" s="36"/>
       <c r="E64" s="25"/>
       <c r="F64" s="25"/>
-      <c r="G64" s="26"/>
-      <c r="H64" s="31"/>
-      <c r="I64" s="27"/>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G64" s="25"/>
+      <c r="H64" s="26"/>
+      <c r="I64" s="31"/>
+      <c r="J64" s="27"/>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="3"/>
       <c r="B65" s="24"/>
       <c r="C65" s="25"/>
       <c r="D65" s="36"/>
       <c r="E65" s="25"/>
       <c r="F65" s="25"/>
-      <c r="G65" s="26"/>
-      <c r="H65" s="31"/>
-      <c r="I65" s="27"/>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G65" s="25"/>
+      <c r="H65" s="26"/>
+      <c r="I65" s="31"/>
+      <c r="J65" s="27"/>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="3"/>
       <c r="B66" s="24"/>
       <c r="C66" s="25"/>
       <c r="D66" s="36"/>
       <c r="E66" s="25"/>
       <c r="F66" s="25"/>
-      <c r="G66" s="26"/>
-      <c r="H66" s="31"/>
-      <c r="I66" s="27"/>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G66" s="25"/>
+      <c r="H66" s="26"/>
+      <c r="I66" s="31"/>
+      <c r="J66" s="27"/>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="3"/>
       <c r="B67" s="24"/>
       <c r="C67" s="25"/>
       <c r="D67" s="36"/>
       <c r="E67" s="25"/>
       <c r="F67" s="25"/>
-      <c r="G67" s="26"/>
-      <c r="H67" s="31"/>
-      <c r="I67" s="27"/>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G67" s="25"/>
+      <c r="H67" s="26"/>
+      <c r="I67" s="31"/>
+      <c r="J67" s="27"/>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="3"/>
       <c r="B68" s="24"/>
       <c r="C68" s="25"/>
       <c r="D68" s="36"/>
       <c r="E68" s="25"/>
       <c r="F68" s="25"/>
-      <c r="G68" s="26"/>
-      <c r="H68" s="31"/>
-      <c r="I68" s="27"/>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G68" s="25"/>
+      <c r="H68" s="26"/>
+      <c r="I68" s="31"/>
+      <c r="J68" s="27"/>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="3"/>
       <c r="B69" s="24"/>
       <c r="C69" s="25"/>
       <c r="D69" s="36"/>
       <c r="E69" s="25"/>
       <c r="F69" s="25"/>
-      <c r="G69" s="26"/>
-      <c r="H69" s="31"/>
-      <c r="I69" s="27"/>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G69" s="25"/>
+      <c r="H69" s="26"/>
+      <c r="I69" s="31"/>
+      <c r="J69" s="27"/>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="3"/>
       <c r="B70" s="24"/>
       <c r="C70" s="25"/>
       <c r="D70" s="36"/>
       <c r="E70" s="25"/>
       <c r="F70" s="25"/>
-      <c r="G70" s="26"/>
-      <c r="H70" s="31"/>
-      <c r="I70" s="27"/>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G70" s="25"/>
+      <c r="H70" s="26"/>
+      <c r="I70" s="31"/>
+      <c r="J70" s="27"/>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="3"/>
       <c r="B71" s="24"/>
       <c r="C71" s="25"/>
       <c r="D71" s="36"/>
       <c r="E71" s="25"/>
       <c r="F71" s="25"/>
-      <c r="G71" s="26"/>
-      <c r="H71" s="31"/>
-      <c r="I71" s="27"/>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G71" s="25"/>
+      <c r="H71" s="26"/>
+      <c r="I71" s="31"/>
+      <c r="J71" s="27"/>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="3"/>
       <c r="B72" s="24"/>
       <c r="C72" s="32"/>
       <c r="D72" s="35"/>
       <c r="E72" s="25"/>
       <c r="F72" s="25"/>
-      <c r="G72" s="26"/>
-      <c r="H72" s="31"/>
-      <c r="I72" s="27"/>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G72" s="25"/>
+      <c r="H72" s="26"/>
+      <c r="I72" s="31"/>
+      <c r="J72" s="27"/>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="3"/>
       <c r="B73" s="24"/>
       <c r="C73" s="25"/>
       <c r="D73" s="37"/>
       <c r="E73" s="25"/>
       <c r="F73" s="25"/>
-      <c r="G73" s="26"/>
-      <c r="H73" s="31"/>
-      <c r="I73" s="27"/>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G73" s="25"/>
+      <c r="H73" s="26"/>
+      <c r="I73" s="31"/>
+      <c r="J73" s="27"/>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="3"/>
       <c r="B74" s="24"/>
       <c r="C74" s="25"/>
       <c r="D74" s="36"/>
       <c r="E74" s="25"/>
       <c r="F74" s="25"/>
-      <c r="G74" s="26"/>
-      <c r="H74" s="31"/>
-      <c r="I74" s="27"/>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G74" s="25"/>
+      <c r="H74" s="26"/>
+      <c r="I74" s="31"/>
+      <c r="J74" s="27"/>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="3"/>
       <c r="B75" s="24"/>
       <c r="C75" s="25"/>
       <c r="D75" s="36"/>
       <c r="E75" s="25"/>
       <c r="F75" s="25"/>
-      <c r="G75" s="26"/>
-      <c r="H75" s="31"/>
-      <c r="I75" s="27"/>
+      <c r="G75" s="25"/>
+      <c r="H75" s="26"/>
+      <c r="I75" s="31"/>
+      <c r="J75" s="27"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
-  <autoFilter ref="A2:I75" xr:uid="{52620AD0-D81A-4707-BF25-930520122703}"/>
+  <autoFilter ref="A2:J75" xr:uid="{52620AD0-D81A-4707-BF25-930520122703}"/>
   <mergeCells count="1">
-    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A1:J1"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H75" xr:uid="{95136ACE-3B61-4F2E-BC2F-785DA5FB4AA4}">
-      <formula1>$AA$7:$AA$8</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I75" xr:uid="{95136ACE-3B61-4F2E-BC2F-785DA5FB4AA4}">
+      <formula1>$AB$7:$AB$8</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G75" xr:uid="{A8A29524-CB88-4A40-9BD1-F8E9BD2459CB}">
-      <formula1>$AA$3:$AA$4</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H75" xr:uid="{A8A29524-CB88-4A40-9BD1-F8E9BD2459CB}">
+      <formula1>$AB$3:$AB$4</formula1>
     </dataValidation>
   </dataValidations>
   <printOptions horizontalCentered="1"/>
@@ -1968,16 +2618,16 @@
       <c r="C1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="48" t="s">
+      <c r="D1" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="49"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="51" t="s">
+      <c r="E1" s="42"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="51"/>
-      <c r="I1" s="52"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="45"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="18">
@@ -1989,60 +2639,60 @@
       <c r="C2" s="15">
         <v>44130</v>
       </c>
-      <c r="D2" s="38" t="s">
+      <c r="D2" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="39"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="39" t="s">
+      <c r="E2" s="47"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="39"/>
-      <c r="I2" s="41"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="49"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="18"/>
       <c r="B3" s="13"/>
       <c r="C3" s="16"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="41"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="49"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="18"/>
       <c r="B4" s="13"/>
       <c r="C4" s="16"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="41"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="49"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="18"/>
       <c r="B5" s="13"/>
       <c r="C5" s="16"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="41"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="49"/>
     </row>
     <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="19"/>
       <c r="B6" s="14"/>
       <c r="C6" s="17"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="43"/>
-      <c r="I6" s="44"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="51"/>
+      <c r="I6" s="52"/>
     </row>
     <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Clean slate incoming inspection log
</commit_message>
<xml_diff>
--- a/dist/modules/data/templates/Incoming Inspection Log.xlsx
+++ b/dist/modules/data/templates/Incoming Inspection Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\austi\Documents\Pragmatic\Projects\DBA-Automation-Tools\dist\modules\data\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FE3C4C9-A680-4E60-AF05-36A64BD54E38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B7ECCC6-03D4-43B6-A485-43DFE20397EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4560" yWindow="1380" windowWidth="19380" windowHeight="12045" xr2:uid="{787A15B7-D0B2-4895-82D1-FA4613D51671}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="27">
   <si>
     <t>Incoming Inspection Log</t>
   </si>
@@ -119,39 +119,6 @@
   </si>
   <si>
     <t>YES</t>
-  </si>
-  <si>
-    <t>CC106014170 S470.1, ETFE 25%GF</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
 </sst>
 </file>
@@ -1075,9 +1042,9 @@
   </sheetPr>
   <dimension ref="A1:AB75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A25" sqref="A25:H50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1778,315 +1745,139 @@
       <c r="J24" s="27"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
-        <v>44927</v>
-      </c>
-      <c r="B25" s="24">
-        <v>100636</v>
-      </c>
-      <c r="C25" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="D25" s="34">
-        <v>123456</v>
-      </c>
-      <c r="E25" s="25">
-        <v>20</v>
-      </c>
-      <c r="F25" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="G25" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="H25" s="26" t="s">
-        <v>26</v>
-      </c>
+      <c r="A25" s="2"/>
+      <c r="B25" s="24"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="34"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="25"/>
+      <c r="H25" s="26"/>
       <c r="I25" s="31"/>
       <c r="J25" s="27"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
-        <v>44927</v>
-      </c>
-      <c r="B26" s="24">
-        <v>100636</v>
-      </c>
-      <c r="C26" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="D26" s="34">
-        <v>123456</v>
-      </c>
-      <c r="E26" s="25">
-        <v>20</v>
-      </c>
-      <c r="F26" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="G26" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="H26" s="26" t="s">
-        <v>26</v>
-      </c>
+      <c r="A26" s="2"/>
+      <c r="B26" s="24"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="34"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="25"/>
+      <c r="G26" s="25"/>
+      <c r="H26" s="26"/>
       <c r="I26" s="31"/>
       <c r="J26" s="27"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
-        <v>44951</v>
-      </c>
-      <c r="B27" s="24">
-        <v>100636</v>
-      </c>
-      <c r="C27" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="D27" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="E27" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="F27" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="G27" s="25">
-        <v>100029</v>
-      </c>
-      <c r="H27" s="26" t="s">
-        <v>29</v>
-      </c>
+      <c r="A27" s="2"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="25"/>
+      <c r="F27" s="25"/>
+      <c r="G27" s="25"/>
+      <c r="H27" s="26"/>
       <c r="I27" s="31"/>
       <c r="J27" s="27"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
-        <v>44951</v>
-      </c>
-      <c r="B28" s="24">
-        <v>100636</v>
-      </c>
-      <c r="C28" s="32" t="s">
-        <v>27</v>
-      </c>
-      <c r="D28" s="34" t="s">
-        <v>30</v>
-      </c>
-      <c r="E28" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="F28" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="G28" s="25">
-        <v>100030</v>
-      </c>
-      <c r="H28" s="26" t="s">
-        <v>29</v>
-      </c>
+      <c r="A28" s="2"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="34"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="26"/>
       <c r="I28" s="31"/>
       <c r="J28" s="27"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
-        <v>44951</v>
-      </c>
-      <c r="B29" s="24">
-        <v>100636</v>
-      </c>
-      <c r="C29" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="D29" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="E29" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="F29" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="G29" s="25">
-        <v>100031</v>
-      </c>
-      <c r="H29" s="26" t="s">
-        <v>29</v>
-      </c>
+      <c r="A29" s="2"/>
+      <c r="B29" s="24"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="34"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="25"/>
+      <c r="H29" s="26"/>
       <c r="I29" s="31"/>
       <c r="J29" s="27"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
-        <v>44951</v>
-      </c>
-      <c r="B30" s="24">
-        <v>100636</v>
-      </c>
-      <c r="C30" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="D30" s="34" t="s">
-        <v>32</v>
-      </c>
-      <c r="E30" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="F30" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="G30" s="25">
-        <v>100041</v>
-      </c>
-      <c r="H30" s="26" t="s">
-        <v>29</v>
-      </c>
+      <c r="A30" s="2"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="34"/>
+      <c r="E30" s="25"/>
+      <c r="F30" s="25"/>
+      <c r="G30" s="25"/>
+      <c r="H30" s="26"/>
       <c r="I30" s="31"/>
       <c r="J30" s="27"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
-        <v>44951</v>
-      </c>
-      <c r="B31" s="28">
-        <v>100636</v>
-      </c>
-      <c r="C31" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="D31" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="E31" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="F31" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="G31" s="25">
-        <v>100042</v>
-      </c>
-      <c r="H31" s="26" t="s">
-        <v>29</v>
-      </c>
+      <c r="A31" s="2"/>
+      <c r="B31" s="28"/>
+      <c r="C31" s="25"/>
+      <c r="D31" s="34"/>
+      <c r="E31" s="25"/>
+      <c r="F31" s="25"/>
+      <c r="G31" s="25"/>
+      <c r="H31" s="26"/>
       <c r="I31" s="31"/>
       <c r="J31" s="27"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
-        <v>44951</v>
-      </c>
-      <c r="B32" s="24">
-        <v>100636</v>
-      </c>
-      <c r="C32" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="D32" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="E32" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="F32" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="G32" s="25">
-        <v>100043</v>
-      </c>
-      <c r="H32" s="26" t="s">
-        <v>29</v>
-      </c>
+      <c r="A32" s="2"/>
+      <c r="B32" s="24"/>
+      <c r="C32" s="25"/>
+      <c r="D32" s="34"/>
+      <c r="E32" s="25"/>
+      <c r="F32" s="25"/>
+      <c r="G32" s="25"/>
+      <c r="H32" s="26"/>
       <c r="I32" s="31"/>
       <c r="J32" s="27"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="2">
-        <v>44951</v>
-      </c>
-      <c r="B33" s="24">
-        <v>100636</v>
-      </c>
-      <c r="C33" s="32" t="s">
-        <v>27</v>
-      </c>
-      <c r="D33" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="E33" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="F33" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="G33" s="25">
-        <v>100044</v>
-      </c>
-      <c r="H33" s="26" t="s">
-        <v>29</v>
-      </c>
+      <c r="A33" s="2"/>
+      <c r="B33" s="24"/>
+      <c r="C33" s="32"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="25"/>
+      <c r="F33" s="25"/>
+      <c r="G33" s="25"/>
+      <c r="H33" s="26"/>
       <c r="I33" s="31"/>
       <c r="J33" s="27"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="2">
-        <v>44951</v>
-      </c>
-      <c r="B34" s="24">
-        <v>100636</v>
-      </c>
-      <c r="C34" s="32" t="s">
-        <v>27</v>
-      </c>
-      <c r="D34" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="E34" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="F34" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="G34" s="25">
-        <v>100045</v>
-      </c>
-      <c r="H34" s="26" t="s">
-        <v>29</v>
-      </c>
+      <c r="A34" s="2"/>
+      <c r="B34" s="24"/>
+      <c r="C34" s="32"/>
+      <c r="D34" s="34"/>
+      <c r="E34" s="25"/>
+      <c r="F34" s="25"/>
+      <c r="G34" s="25"/>
+      <c r="H34" s="26"/>
       <c r="I34" s="31"/>
       <c r="J34" s="27"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="2">
-        <v>44951</v>
-      </c>
-      <c r="B35" s="24">
-        <v>100636</v>
-      </c>
-      <c r="C35" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="D35" s="34" t="s">
-        <v>36</v>
-      </c>
-      <c r="E35" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="F35" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="G35" s="25">
-        <v>100046</v>
-      </c>
-      <c r="H35" s="26" t="s">
-        <v>37</v>
-      </c>
+      <c r="A35" s="2"/>
+      <c r="B35" s="24"/>
+      <c r="C35" s="25"/>
+      <c r="D35" s="34"/>
+      <c r="E35" s="25"/>
+      <c r="F35" s="25"/>
+      <c r="G35" s="25"/>
+      <c r="H35" s="26"/>
       <c r="I35" s="31"/>
       <c r="J35" s="27"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="3"/>
+      <c r="A36" s="2"/>
       <c r="B36" s="24"/>
       <c r="C36" s="25"/>
       <c r="D36" s="34"/>
@@ -2098,7 +1889,7 @@
       <c r="J36" s="27"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="3"/>
+      <c r="A37" s="2"/>
       <c r="B37" s="24"/>
       <c r="C37" s="25"/>
       <c r="D37" s="34"/>
@@ -2110,7 +1901,7 @@
       <c r="J37" s="27"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="3"/>
+      <c r="A38" s="2"/>
       <c r="B38" s="24"/>
       <c r="C38" s="25"/>
       <c r="D38" s="34"/>
@@ -2122,7 +1913,7 @@
       <c r="J38" s="27"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="3"/>
+      <c r="A39" s="2"/>
       <c r="B39" s="24"/>
       <c r="C39" s="25"/>
       <c r="D39" s="34"/>
@@ -2134,7 +1925,7 @@
       <c r="J39" s="27"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="3"/>
+      <c r="A40" s="2"/>
       <c r="B40" s="24"/>
       <c r="C40" s="25"/>
       <c r="D40" s="34"/>
@@ -2146,7 +1937,7 @@
       <c r="J40" s="27"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="3"/>
+      <c r="A41" s="2"/>
       <c r="B41" s="24"/>
       <c r="C41" s="25"/>
       <c r="D41" s="34"/>
@@ -2158,7 +1949,7 @@
       <c r="J41" s="27"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="3"/>
+      <c r="A42" s="2"/>
       <c r="B42" s="24"/>
       <c r="C42" s="32"/>
       <c r="D42" s="34"/>
@@ -2170,7 +1961,7 @@
       <c r="J42" s="27"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="3"/>
+      <c r="A43" s="2"/>
       <c r="B43" s="24"/>
       <c r="C43" s="25"/>
       <c r="D43" s="35"/>
@@ -2182,7 +1973,7 @@
       <c r="J43" s="27"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="3"/>
+      <c r="A44" s="2"/>
       <c r="B44" s="24"/>
       <c r="C44" s="25"/>
       <c r="D44" s="34"/>
@@ -2194,7 +1985,7 @@
       <c r="J44" s="27"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="3"/>
+      <c r="A45" s="2"/>
       <c r="B45" s="24"/>
       <c r="C45" s="25"/>
       <c r="D45" s="34"/>
@@ -2206,7 +1997,7 @@
       <c r="J45" s="27"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="3"/>
+      <c r="A46" s="2"/>
       <c r="B46" s="24"/>
       <c r="C46" s="25"/>
       <c r="D46" s="34"/>
@@ -2218,7 +2009,7 @@
       <c r="J46" s="27"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="3"/>
+      <c r="A47" s="2"/>
       <c r="B47" s="24"/>
       <c r="C47" s="25"/>
       <c r="D47" s="34"/>
@@ -2230,7 +2021,7 @@
       <c r="J47" s="27"/>
     </row>
     <row r="48" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="3"/>
+      <c r="A48" s="2"/>
       <c r="B48" s="24"/>
       <c r="C48" s="32"/>
       <c r="D48" s="34"/>
@@ -2242,7 +2033,7 @@
       <c r="J48" s="27"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="3"/>
+      <c r="A49" s="2"/>
       <c r="B49" s="24"/>
       <c r="C49" s="25"/>
       <c r="D49" s="36"/>
@@ -2254,7 +2045,7 @@
       <c r="J49" s="27"/>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="3"/>
+      <c r="A50" s="2"/>
       <c r="B50" s="24"/>
       <c r="C50" s="32"/>
       <c r="D50" s="35"/>

</xml_diff>